<commit_message>
updated code for SF calibration
</commit_message>
<xml_diff>
--- a/sim/calibrate_result_SF.xlsx
+++ b/sim/calibrate_result_SF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZihanWei\Documents\Stanford\Course\2020Spring\218Z\model-Jun25\simulator\sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423B5682-73B8-427B-9513-24D15BFB8B10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E1EDA7-0FF2-415C-95F9-A1EFE35C56DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>n_init_samples</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>downsample</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>subdivide offices</t>
+  </si>
+  <si>
+    <t>0.2?</t>
   </si>
 </sst>
 </file>
@@ -65,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -99,7 +108,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
@@ -393,9 +402,11 @@
     <col min="3" max="3" width="10.734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.89453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.41796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.89453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -429,8 +440,11 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>43894</v>
       </c>
@@ -463,6 +477,73 @@
       </c>
       <c r="K2">
         <v>0.65943020582199097</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2">
+        <v>43894</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43909</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
+      </c>
+      <c r="G3">
+        <v>1.51399550959467E-2</v>
+      </c>
+      <c r="H3">
+        <v>0.111006572842597</v>
+      </c>
+      <c r="I3">
+        <v>4.3372111395001403E-3</v>
+      </c>
+      <c r="J3">
+        <v>0.23195971548557201</v>
+      </c>
+      <c r="K3">
+        <v>1.35917520523071</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1">
+        <v>43894</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43945</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="H4">
+        <v>0.04</v>
+      </c>
+      <c r="I4">
+        <v>0.1</v>
+      </c>
+      <c r="J4">
+        <v>0.04</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>